<commit_message>
pull down changes to local comp
</commit_message>
<xml_diff>
--- a/ocr-workouts/workouts.xlsx
+++ b/ocr-workouts/workouts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6320" yWindow="1760" windowWidth="21500" windowHeight="16660"/>
+    <workbookView xWindow="6320" yWindow="1340" windowWidth="21500" windowHeight="16660"/>
   </bookViews>
   <sheets>
     <sheet name="OCR Workouts" sheetId="1" r:id="rId1"/>
@@ -643,12 +643,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -659,11 +653,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -692,27 +692,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1029,29 +1008,29 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R1048517"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="6"/>
-    <col min="2" max="2" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="10.83203125" style="6"/>
-    <col min="8" max="8" width="14.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="10.83203125" style="6"/>
-    <col min="12" max="17" width="10.83203125" style="8"/>
-    <col min="18" max="18" width="18.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="2" max="2" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.83203125" style="4"/>
+    <col min="8" max="8" width="14.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.83203125" style="4"/>
+    <col min="12" max="17" width="10.83203125" style="6"/>
+    <col min="18" max="18" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>174</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1066,1999 +1045,1999 @@
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="4" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="5" t="s">
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C2" s="6">
+    <row r="2" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="L2" s="8" t="s">
+      <c r="H2" s="5"/>
+      <c r="L2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="7"/>
-      <c r="L3" s="8" t="s">
+      <c r="G3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="L3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="7"/>
-      <c r="L4" s="8" t="s">
+      <c r="G4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="L4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="A5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" s="4">
         <v>2</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="7"/>
-      <c r="L5" s="8" t="s">
+      <c r="F5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="L5" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="L6" s="8" t="s">
+      <c r="G6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="L6" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="L7" s="8" t="s">
+      <c r="G7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="L7" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="L8" s="8" t="s">
+      <c r="G8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="L8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D9" s="7" t="s">
+    <row r="9" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="L9" s="8" t="s">
+      <c r="F9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="L9" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C10" s="6">
+    <row r="10" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" s="4">
         <v>3</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="7"/>
-      <c r="L10" s="8" t="s">
+      <c r="G10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="L10" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="7" t="s">
+    <row r="11" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="7"/>
-      <c r="L11" s="8" t="s">
+      <c r="F11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="L11" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="7"/>
-      <c r="L12" s="8" t="s">
+      <c r="G12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="L12" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="L13" s="8" t="s">
+      <c r="H13" s="5"/>
+      <c r="L13" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C14" s="6">
+    <row r="14" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="4">
         <v>4</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="7"/>
-      <c r="L14" s="8" t="s">
+      <c r="H14" s="5"/>
+      <c r="L14" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="7" t="s">
+    <row r="15" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="7" t="s">
+      <c r="F15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="L15" s="8" t="s">
+      <c r="H15" s="5"/>
+      <c r="L15" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="L16" s="8" t="s">
+      <c r="H16" s="5"/>
+      <c r="L16" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C17" s="6">
+      <c r="A17" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" s="4">
         <v>5</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="F17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="7" t="s">
+    <row r="18" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="7" t="s">
+      <c r="F18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="7"/>
-      <c r="L18" s="8" t="s">
+      <c r="H18" s="5"/>
+      <c r="L18" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="L19" s="8" t="s">
+      <c r="H19" s="5"/>
+      <c r="L19" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C20" s="6">
+    <row r="20" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="4">
         <v>6</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="7"/>
-      <c r="L20" s="8" t="s">
+      <c r="H20" s="5"/>
+      <c r="L20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="R20" s="6" t="s">
+      <c r="R20" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H21" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="L21" s="8" t="s">
+      <c r="L21" s="6" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="7"/>
-      <c r="L22" s="8" t="s">
+      <c r="H22" s="5"/>
+      <c r="L22" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D23" s="7" t="s">
+    <row r="23" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D23" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="7" t="s">
+      <c r="F23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H23" s="7"/>
-      <c r="L23" s="8" t="s">
+      <c r="H23" s="5"/>
+      <c r="L23" s="6" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H24" s="7"/>
-      <c r="L24" s="8" t="s">
+      <c r="H24" s="5"/>
+      <c r="L24" s="6" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H25" s="7"/>
-      <c r="L25" s="8" t="s">
+      <c r="H25" s="5"/>
+      <c r="L25" s="6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D26" s="7" t="s">
+    <row r="26" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D26" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="7" t="s">
+      <c r="F26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H26" s="7"/>
-      <c r="L26" s="8" t="s">
+      <c r="H26" s="5"/>
+      <c r="L26" s="6" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C27" s="6">
+      <c r="A27" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C27" s="4">
         <v>7</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="7" t="s">
+      <c r="F27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="7"/>
-      <c r="L27" s="8" t="s">
+      <c r="H27" s="5"/>
+      <c r="L27" s="6" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D28" s="7"/>
-      <c r="E28" s="7" t="s">
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C29" s="6">
-        <v>8</v>
-      </c>
-      <c r="D29" s="7" t="s">
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" s="4">
+        <v>8</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" s="7" t="s">
+      <c r="E29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G29" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="7"/>
-      <c r="L29" s="8" t="s">
+      <c r="G29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="L29" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D30" s="7" t="s">
+    <row r="30" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="7"/>
-      <c r="L30" s="8" t="s">
+      <c r="E30" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="L30" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" s="7" t="s">
+      <c r="E31" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="7"/>
-      <c r="L31" s="8" t="s">
+      <c r="G31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="5"/>
+      <c r="L31" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="R31" s="6" t="s">
+      <c r="R31" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D32" s="7" t="s">
+    <row r="32" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D32" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" s="7"/>
-      <c r="L32" s="8" t="s">
+      <c r="E32" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="5"/>
+      <c r="L32" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="R32" s="6" t="s">
+      <c r="R32" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F33" s="7" t="s">
+      <c r="E33" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="7"/>
-      <c r="L33" s="8" t="s">
+      <c r="G33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="5"/>
+      <c r="L33" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="R33" s="6" t="s">
+      <c r="R33" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D34" s="7" t="s">
+    <row r="34" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D34" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="7"/>
-      <c r="L34" s="8" t="s">
+      <c r="E34" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="L34" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="R34" s="6" t="s">
+      <c r="R34" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C35" s="6">
+      <c r="A35" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="4">
         <v>9</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="7"/>
-      <c r="L35" s="8" t="s">
+      <c r="E35" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="5"/>
+      <c r="L35" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F36" s="7" t="s">
+      <c r="E36" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="7"/>
-      <c r="L36" s="8" t="s">
+      <c r="G36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="5"/>
+      <c r="L36" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F37" s="7" t="s">
+      <c r="E37" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G37" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="7"/>
-      <c r="L37" s="8" t="s">
+      <c r="G37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="5"/>
+      <c r="L37" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F38" s="7" t="s">
+      <c r="E38" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H38" s="7"/>
-      <c r="L38" s="8" t="s">
+      <c r="G38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="5"/>
+      <c r="L38" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D39" s="7" t="s">
+    <row r="39" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D39" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" s="7"/>
-      <c r="L39" s="8" t="s">
+      <c r="E39" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="5"/>
+      <c r="L39" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C40" s="6">
+      <c r="A40" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C40" s="4">
         <v>10</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H40" s="7"/>
-      <c r="L40" s="8" t="s">
+      <c r="E40" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" s="5"/>
+      <c r="L40" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F41" s="7" t="s">
+      <c r="E41" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" s="7"/>
-      <c r="L41" s="8" t="s">
+      <c r="G41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" s="5"/>
+      <c r="L41" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D42" s="7" t="s">
+    <row r="42" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D42" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" s="7"/>
-      <c r="L42" s="8" t="s">
+      <c r="E42" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H42" s="5"/>
+      <c r="L42" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F43" s="7" t="s">
+      <c r="E43" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G43" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H43" s="7"/>
-      <c r="L43" s="8" t="s">
+      <c r="G43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" s="5"/>
+      <c r="L43" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E44" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F44" s="7" t="s">
+      <c r="E44" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F44" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" s="7"/>
-      <c r="L44" s="8" t="s">
+      <c r="G44" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="5"/>
+      <c r="L44" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D45" s="7" t="s">
+    <row r="45" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D45" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E45" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H45" s="7"/>
-      <c r="L45" s="8" t="s">
+      <c r="E45" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" s="5"/>
+      <c r="L45" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E46" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F46" s="7" t="s">
+      <c r="E46" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G46" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H46" s="7"/>
-      <c r="L46" s="8" t="s">
+      <c r="G46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="5"/>
+      <c r="L46" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D47" s="7" t="s">
+    <row r="47" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D47" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H47" s="7"/>
-      <c r="L47" s="8" t="s">
+      <c r="E47" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" s="5"/>
+      <c r="L47" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C48" s="6">
+      <c r="A48" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C48" s="4">
         <v>11</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E48" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H48" s="7"/>
-      <c r="L48" s="8" t="s">
+      <c r="E48" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" s="5"/>
+      <c r="L48" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E49" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F49" s="7" t="s">
+      <c r="E49" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G49" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H49" s="7"/>
-      <c r="L49" s="8" t="s">
+      <c r="G49" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" s="5"/>
+      <c r="L49" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E50" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F50" s="7" t="s">
+      <c r="E50" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G50" s="7" t="s">
+      <c r="G50" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H50" s="7"/>
-      <c r="L50" s="8" t="s">
+      <c r="H50" s="5"/>
+      <c r="L50" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C51" s="6">
-        <v>12</v>
-      </c>
-      <c r="D51" s="7" t="s">
+    <row r="51" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C51" s="4">
+        <v>12</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F51" s="7" t="s">
+      <c r="E51" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G51" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H51" s="7"/>
-      <c r="L51" s="8" t="s">
+      <c r="G51" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" s="5"/>
+      <c r="L51" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D52" s="7" t="s">
+    <row r="52" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D52" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E52" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H52" s="7"/>
-      <c r="L52" s="8" t="s">
+      <c r="E52" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="5"/>
+      <c r="L52" s="6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C53" s="6">
+    <row r="53" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C53" s="4">
         <v>13</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E53" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F53" s="7" t="s">
+      <c r="E53" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G53" s="7" t="s">
+      <c r="G53" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H53" s="7"/>
-      <c r="L53" s="8" t="s">
+      <c r="H53" s="5"/>
+      <c r="L53" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D54" s="7" t="s">
+    <row r="54" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D54" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E54" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G54" s="7" t="s">
+      <c r="E54" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H54" s="7"/>
-      <c r="L54" s="8" t="s">
+      <c r="H54" s="5"/>
+      <c r="L54" s="6" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E55" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F55" s="7" t="s">
+      <c r="E55" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G55" s="7" t="s">
+      <c r="G55" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H55" s="7"/>
-      <c r="L55" s="8" t="s">
+      <c r="H55" s="5"/>
+      <c r="L55" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D56" s="7" t="s">
+    <row r="56" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D56" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E56" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G56" s="7" t="s">
+      <c r="E56" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H56" s="7"/>
-      <c r="L56" s="8" t="s">
+      <c r="H56" s="5"/>
+      <c r="L56" s="6" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E57" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F57" s="7" t="s">
+      <c r="E57" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="L57" s="8" t="s">
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="L57" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D58" s="7" t="s">
+    <row r="58" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D58" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E58" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="L58" s="8" t="s">
+      <c r="E58" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="L58" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E59" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F59" s="7" t="s">
+      <c r="E59" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F59" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-      <c r="L59" s="8" t="s">
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="L59" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="R59" s="6" t="s">
+      <c r="R59" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D60" s="7" t="s">
+    <row r="60" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D60" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E60" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-      <c r="L60" s="8" t="s">
+      <c r="E60" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="L60" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="R60" s="6" t="s">
+      <c r="R60" s="4" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E61" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F61" s="7" t="s">
+      <c r="E61" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
-      <c r="L61" s="8" t="s">
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="L61" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D62" s="7" t="s">
+    <row r="62" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D62" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E62" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="L62" s="8" t="s">
+      <c r="E62" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="L62" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D63" s="7" t="s">
+    <row r="63" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D63" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E63" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-      <c r="L63" s="8" t="s">
+      <c r="E63" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="L63" s="6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B64" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C64" s="6">
+    <row r="64" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C64" s="4">
         <v>14</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="E64" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F64" s="7" t="s">
+      <c r="E64" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F64" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G64" s="7" t="s">
+      <c r="G64" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H64" s="7"/>
-      <c r="L64" s="8" t="s">
+      <c r="H64" s="5"/>
+      <c r="L64" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D65" s="7" t="s">
+    <row r="65" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D65" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E65" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F65" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
-      <c r="L65" s="8" t="s">
+      <c r="E65" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="L65" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D66" s="7"/>
-      <c r="E66" s="7" t="s">
+      <c r="D66" s="5"/>
+      <c r="E66" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
-    </row>
-    <row r="67" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C67" s="6">
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C67" s="4">
         <v>15</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="E67" s="7" t="s">
+      <c r="E67" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F67" s="7" t="s">
+      <c r="F67" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G67" s="7" t="s">
+      <c r="G67" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="H67" s="7"/>
-      <c r="L67" s="8" t="s">
+      <c r="H67" s="5"/>
+      <c r="L67" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B68" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C68" s="6">
+    <row r="68" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C68" s="4">
         <v>16</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E68" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F68" s="7" t="s">
+      <c r="F68" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G68" s="7" t="s">
+      <c r="G68" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="H68" s="7" t="s">
+      <c r="H68" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="L68" s="8" t="s">
+      <c r="L68" s="6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B69" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C69" s="6">
+    <row r="69" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C69" s="4">
         <v>17</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E69" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F69" s="7" t="s">
+      <c r="F69" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G69" s="7" t="s">
+      <c r="G69" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H69" s="7"/>
-      <c r="L69" s="8" t="s">
+      <c r="H69" s="5"/>
+      <c r="L69" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="R69" s="6" t="s">
+      <c r="R69" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B70" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C70" s="6">
+    <row r="70" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C70" s="4">
         <v>18</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E70" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="F70" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G70" s="7" t="s">
+      <c r="G70" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H70" s="7" t="s">
+      <c r="H70" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="I70" s="6" t="s">
+      <c r="I70" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="L70" s="8" t="s">
+      <c r="L70" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D71" s="7" t="s">
+    <row r="71" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D71" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G71" s="7" t="s">
+      <c r="E71" s="5"/>
+      <c r="F71" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G71" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="H71" s="7" t="s">
+      <c r="H71" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="I71" s="6" t="s">
+      <c r="I71" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="L71" s="8" t="s">
+      <c r="L71" s="6" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B72" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C72" s="6">
+      <c r="A72" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C72" s="4">
         <v>19</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E72" s="7" t="s">
+      <c r="E72" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F72" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G72" s="7"/>
-      <c r="H72" s="7" t="s">
+      <c r="F72" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="J72" s="6" t="s">
+      <c r="J72" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L72" s="8" t="s">
+      <c r="L72" s="6" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C73" s="6">
+    <row r="73" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C73" s="4">
         <v>20</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="E73" s="7" t="s">
+      <c r="E73" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F73" s="7" t="s">
+      <c r="F73" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G73" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H73" s="7"/>
-      <c r="L73" s="8" t="s">
+      <c r="G73" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H73" s="5"/>
+      <c r="L73" s="6" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B74" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C74" s="6">
+    <row r="74" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C74" s="4">
         <v>21</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D74" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="E74" s="7" t="s">
+      <c r="E74" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F74" s="7" t="s">
+      <c r="F74" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G74" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H74" s="7"/>
-      <c r="L74" s="8" t="s">
+      <c r="G74" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H74" s="5"/>
+      <c r="L74" s="6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D75" s="7" t="s">
+    <row r="75" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D75" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="E75" s="7" t="s">
+      <c r="E75" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F75" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G75" s="7" t="s">
+      <c r="F75" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G75" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="H75" s="7" t="s">
+      <c r="H75" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="J75" s="6" t="s">
+      <c r="J75" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L75" s="8" t="s">
+      <c r="L75" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B76" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C76" s="6">
+    <row r="76" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C76" s="4">
         <v>22</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D76" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E76" s="7" t="s">
+      <c r="E76" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F76" s="7" t="s">
+      <c r="F76" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G76" s="7" t="s">
+      <c r="G76" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H76" s="7" t="s">
+      <c r="H76" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="L76" s="8" t="s">
+      <c r="L76" s="6" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="77" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C77" s="6">
+      <c r="A77" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C77" s="4">
         <v>23</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E77" s="7" t="s">
+      <c r="E77" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F77" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G77" s="7" t="s">
+      <c r="F77" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G77" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="H77" s="7" t="s">
+      <c r="H77" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="I77" s="6" t="s">
+      <c r="I77" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="J77" s="6" t="s">
+      <c r="J77" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L77" s="8" t="s">
+      <c r="L77" s="6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D78" s="7" t="s">
+    <row r="78" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D78" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="E78" s="7" t="s">
+      <c r="E78" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F78" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G78" s="7" t="s">
+      <c r="F78" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G78" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H78" s="7"/>
-      <c r="L78" s="8" t="s">
+      <c r="H78" s="5"/>
+      <c r="L78" s="6" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B79" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C79" s="6">
+      <c r="A79" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C79" s="4">
         <v>24</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D79" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="E79" s="7" t="s">
+      <c r="E79" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F79" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G79" s="7"/>
-      <c r="H79" s="7" t="s">
+      <c r="F79" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="I79" s="6" t="s">
+      <c r="I79" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="J79" s="6" t="s">
+      <c r="J79" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L79" s="8" t="s">
+      <c r="L79" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C80" s="6">
+    <row r="80" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" s="4">
         <v>25</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D80" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E80" s="7" t="s">
+      <c r="E80" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F80" s="7" t="s">
+      <c r="F80" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G80" s="7" t="s">
+      <c r="G80" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H80" s="7" t="s">
+      <c r="H80" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="L80" s="8" t="s">
+      <c r="L80" s="6" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="81" spans="2:8" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="10"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="7"/>
-      <c r="F81" s="7"/>
-      <c r="G81" s="7"/>
-      <c r="H81" s="7"/>
+      <c r="B81" s="8"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
     </row>
     <row r="82" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
-      <c r="G82" s="7"/>
-      <c r="H82" s="7"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
     </row>
     <row r="83" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D83" s="7"/>
-      <c r="E83" s="7"/>
-      <c r="F83" s="7"/>
-      <c r="G83" s="7"/>
-      <c r="H83" s="7"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
     </row>
     <row r="84" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D84" s="7"/>
-      <c r="E84" s="7"/>
-      <c r="F84" s="7"/>
-      <c r="G84" s="7"/>
-      <c r="H84" s="7"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
     </row>
     <row r="85" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D85" s="7"/>
-      <c r="E85" s="7"/>
-      <c r="F85" s="7"/>
-      <c r="G85" s="7"/>
-      <c r="H85" s="7"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
     </row>
     <row r="86" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D86" s="7"/>
-      <c r="E86" s="7"/>
-      <c r="F86" s="7"/>
-      <c r="G86" s="7"/>
-      <c r="H86" s="7"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
     </row>
     <row r="87" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D87" s="7"/>
-      <c r="E87" s="7"/>
-      <c r="F87" s="7"/>
-      <c r="G87" s="7"/>
-      <c r="H87" s="7"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
     </row>
     <row r="88" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D88" s="7"/>
-      <c r="E88" s="7"/>
-      <c r="F88" s="7"/>
-      <c r="G88" s="7"/>
-      <c r="H88" s="7"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
     </row>
     <row r="89" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D89" s="7"/>
-      <c r="E89" s="7"/>
-      <c r="F89" s="7"/>
-      <c r="G89" s="7"/>
-      <c r="H89" s="7"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
     </row>
     <row r="90" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D90" s="7"/>
-      <c r="E90" s="7"/>
-      <c r="F90" s="7"/>
-      <c r="G90" s="7"/>
-      <c r="H90" s="7"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
     </row>
     <row r="91" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D91" s="7"/>
-      <c r="E91" s="7"/>
-      <c r="F91" s="7"/>
-      <c r="G91" s="7"/>
-      <c r="H91" s="7"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5"/>
     </row>
     <row r="92" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D92" s="7"/>
-      <c r="E92" s="7"/>
-      <c r="F92" s="7"/>
-      <c r="G92" s="7"/>
-      <c r="H92" s="7"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
     </row>
     <row r="93" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D93" s="7"/>
-      <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="7"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
     </row>
     <row r="94" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D94" s="7"/>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
     </row>
     <row r="95" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D95" s="7"/>
-      <c r="E95" s="7"/>
-      <c r="F95" s="7"/>
-      <c r="G95" s="7"/>
-      <c r="H95" s="7"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
     </row>
     <row r="96" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D96" s="7"/>
-      <c r="E96" s="7"/>
-      <c r="F96" s="7"/>
-      <c r="G96" s="7"/>
-      <c r="H96" s="7"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
     </row>
     <row r="97" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D97" s="7"/>
-      <c r="E97" s="7"/>
-      <c r="F97" s="7"/>
-      <c r="G97" s="7"/>
-      <c r="H97" s="7"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5"/>
     </row>
     <row r="98" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D98" s="7"/>
-      <c r="E98" s="7"/>
-      <c r="F98" s="7"/>
-      <c r="G98" s="7"/>
-      <c r="H98" s="7"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
     </row>
     <row r="99" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D99" s="7"/>
-      <c r="E99" s="7"/>
-      <c r="F99" s="7"/>
-      <c r="G99" s="7"/>
-      <c r="H99" s="7"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5"/>
     </row>
     <row r="100" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D100" s="7"/>
-      <c r="E100" s="7"/>
-      <c r="F100" s="7"/>
-      <c r="G100" s="7"/>
-      <c r="H100" s="7"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
     </row>
     <row r="101" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D101" s="7"/>
-      <c r="E101" s="7"/>
-      <c r="F101" s="7"/>
-      <c r="G101" s="7"/>
-      <c r="H101" s="7"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+      <c r="G101" s="5"/>
+      <c r="H101" s="5"/>
     </row>
     <row r="102" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D102" s="7"/>
-      <c r="E102" s="7"/>
-      <c r="F102" s="7"/>
-      <c r="G102" s="7"/>
-      <c r="H102" s="7"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
     </row>
     <row r="103" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D103" s="7"/>
-      <c r="E103" s="7"/>
-      <c r="F103" s="7"/>
-      <c r="G103" s="7"/>
-      <c r="H103" s="7"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
+      <c r="H103" s="5"/>
     </row>
     <row r="104" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D104" s="7"/>
-      <c r="E104" s="7"/>
-      <c r="F104" s="7"/>
-      <c r="G104" s="7"/>
-      <c r="H104" s="7"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
+      <c r="G104" s="5"/>
+      <c r="H104" s="5"/>
     </row>
     <row r="105" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D105" s="7"/>
-      <c r="E105" s="7"/>
-      <c r="F105" s="7"/>
-      <c r="G105" s="7"/>
-      <c r="H105" s="7"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5"/>
     </row>
     <row r="106" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D106" s="7"/>
-      <c r="E106" s="7"/>
-      <c r="F106" s="7"/>
-      <c r="G106" s="7"/>
-      <c r="H106" s="7"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="5"/>
+      <c r="H106" s="5"/>
     </row>
     <row r="107" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D107" s="7"/>
-      <c r="E107" s="7"/>
-      <c r="F107" s="7"/>
-      <c r="G107" s="7"/>
-      <c r="H107" s="7"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="5"/>
     </row>
     <row r="108" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D108" s="7"/>
-      <c r="E108" s="7"/>
-      <c r="F108" s="7"/>
-      <c r="G108" s="7"/>
-      <c r="H108" s="7"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="5"/>
     </row>
     <row r="109" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D109" s="7"/>
-      <c r="E109" s="7"/>
-      <c r="F109" s="7"/>
-      <c r="G109" s="7"/>
-      <c r="H109" s="7"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5"/>
     </row>
     <row r="110" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D110" s="7"/>
-      <c r="E110" s="7"/>
-      <c r="F110" s="7"/>
-      <c r="G110" s="7"/>
-      <c r="H110" s="7"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="5"/>
+      <c r="G110" s="5"/>
+      <c r="H110" s="5"/>
     </row>
     <row r="111" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D111" s="7"/>
-      <c r="E111" s="7"/>
-      <c r="F111" s="7"/>
-      <c r="G111" s="7"/>
-      <c r="H111" s="7"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5"/>
+      <c r="G111" s="5"/>
+      <c r="H111" s="5"/>
     </row>
     <row r="112" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D112" s="7"/>
-      <c r="E112" s="7"/>
-      <c r="F112" s="7"/>
-      <c r="G112" s="7"/>
-      <c r="H112" s="7"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="5"/>
+      <c r="G112" s="5"/>
+      <c r="H112" s="5"/>
     </row>
     <row r="113" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D113" s="7"/>
-      <c r="E113" s="7"/>
-      <c r="F113" s="7"/>
-      <c r="G113" s="7"/>
-      <c r="H113" s="7"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="5"/>
+      <c r="G113" s="5"/>
+      <c r="H113" s="5"/>
     </row>
     <row r="114" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D114" s="7"/>
-      <c r="E114" s="7"/>
-      <c r="F114" s="7"/>
-      <c r="G114" s="7"/>
-      <c r="H114" s="7"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="5"/>
+      <c r="G114" s="5"/>
+      <c r="H114" s="5"/>
     </row>
     <row r="115" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D115" s="7"/>
-      <c r="E115" s="7"/>
-      <c r="F115" s="7"/>
-      <c r="G115" s="7"/>
-      <c r="H115" s="7"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
     </row>
     <row r="116" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D116" s="7"/>
-      <c r="E116" s="7"/>
-      <c r="F116" s="7"/>
-      <c r="G116" s="7"/>
-      <c r="H116" s="7"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="5"/>
     </row>
     <row r="117" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D117" s="7"/>
-      <c r="E117" s="7"/>
-      <c r="F117" s="7"/>
-      <c r="G117" s="7"/>
-      <c r="H117" s="7"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="5"/>
+      <c r="G117" s="5"/>
+      <c r="H117" s="5"/>
     </row>
     <row r="118" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D118" s="7"/>
-      <c r="E118" s="7"/>
-      <c r="F118" s="7"/>
-      <c r="G118" s="7"/>
-      <c r="H118" s="7"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="5"/>
+      <c r="G118" s="5"/>
+      <c r="H118" s="5"/>
     </row>
     <row r="119" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D119" s="7"/>
-      <c r="E119" s="7"/>
-      <c r="F119" s="7"/>
-      <c r="G119" s="7"/>
-      <c r="H119" s="7"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5"/>
+      <c r="G119" s="5"/>
+      <c r="H119" s="5"/>
     </row>
     <row r="120" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D120" s="7"/>
-      <c r="E120" s="7"/>
-      <c r="F120" s="7"/>
-      <c r="G120" s="7"/>
-      <c r="H120" s="7"/>
+      <c r="D120" s="5"/>
+      <c r="E120" s="5"/>
+      <c r="F120" s="5"/>
+      <c r="G120" s="5"/>
+      <c r="H120" s="5"/>
     </row>
     <row r="121" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D121" s="7"/>
-      <c r="E121" s="7"/>
-      <c r="F121" s="7"/>
-      <c r="G121" s="7"/>
-      <c r="H121" s="7"/>
+      <c r="D121" s="5"/>
+      <c r="E121" s="5"/>
+      <c r="F121" s="5"/>
+      <c r="G121" s="5"/>
+      <c r="H121" s="5"/>
     </row>
     <row r="1048517" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1048517" s="9"/>
+      <c r="B1048517" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:V81">
-    <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="40-60"/>
+      </filters>
     </filterColumn>
     <filterColumn colId="6" showButton="0"/>
     <filterColumn colId="7" showButton="0"/>
@@ -3069,9 +3048,6 @@
     <filterColumn colId="13" showButton="0"/>
     <filterColumn colId="14" showButton="0"/>
     <filterColumn colId="15" showButton="0"/>
-    <sortState ref="A2:R80">
-      <sortCondition ref="C1:C81"/>
-    </sortState>
   </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="G1:K1"/>

</xml_diff>

<commit_message>
rmv murph duplication in join table
</commit_message>
<xml_diff>
--- a/ocr-workouts/workouts.xlsx
+++ b/ocr-workouts/workouts.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamkuhn/workspace/bootcamp/workout-generator/ocr-workouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C8E6441C-FD1B-7B4F-8F22-91F095386AB2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6320" yWindow="1340" windowWidth="21500" windowHeight="16660"/>
+    <workbookView xWindow="11980" yWindow="460" windowWidth="21500" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OCR Workouts" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="176">
   <si>
     <t>ID</t>
   </si>
@@ -245,9 +246,6 @@
     <t>10 min warm up, 3x 10 min Hard, 90s rest, 10 min cool down</t>
   </si>
   <si>
-    <t>Temp-Hill 2</t>
-  </si>
-  <si>
     <t>Temp-Hill 1</t>
   </si>
   <si>
@@ -524,9 +522,6 @@
     <t>BW Legs</t>
   </si>
   <si>
-    <t>3x 20 Reverse Lunge - 15 toes 2 air, E2MOM for 10 min: 1 min wall sit - 1 min plank, 4x 10 step ups - 10 burpee box</t>
-  </si>
-  <si>
     <t>Chop-it-up</t>
   </si>
   <si>
@@ -555,12 +550,18 @@
   </si>
   <si>
     <t>kettlebell/db</t>
+  </si>
+  <si>
+    <t>Tempo-Hill 2</t>
+  </si>
+  <si>
+    <t>3x 20 Reverse Lunge - 15 toes 2 air, E2MOM for 10 min: 1 min wall sit - 1 min plank, 4x 10 step ups - 10 burpee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1004,12 +1005,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R1048517"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I82" sqref="I82"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1028,10 +1029,10 @@
   <sheetData>
     <row r="1" spans="1:18" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>172</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>174</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1064,12 +1065,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -1084,7 +1085,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H2" s="5"/>
       <c r="L2" s="6" t="s">
@@ -1129,10 +1130,10 @@
     </row>
     <row r="5" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C5" s="4">
         <v>2</v>
@@ -1209,6 +1210,15 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" s="4">
+        <v>26</v>
+      </c>
       <c r="D9" s="5" t="s">
         <v>32</v>
       </c>
@@ -1226,12 +1236,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C10" s="4">
         <v>3</v>
@@ -1254,6 +1264,15 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="4">
+        <v>27</v>
+      </c>
       <c r="D11" s="5" t="s">
         <v>24</v>
       </c>
@@ -1307,12 +1326,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C14" s="4">
         <v>4</v>
@@ -1335,6 +1354,15 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="8">
+        <v>28</v>
+      </c>
       <c r="D15" s="5" t="s">
         <v>23</v>
       </c>
@@ -1372,16 +1400,16 @@
     </row>
     <row r="17" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C17" s="4">
         <v>5</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>5</v>
@@ -1393,13 +1421,22 @@
         <v>18</v>
       </c>
       <c r="H17" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="L17" s="6" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="18" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="4">
+        <v>29</v>
+      </c>
       <c r="D18" s="5" t="s">
         <v>38</v>
       </c>
@@ -1435,12 +1472,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C20" s="4">
         <v>6</v>
@@ -1467,27 +1504,27 @@
     </row>
     <row r="21" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D22" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>5</v>
@@ -1500,30 +1537,39 @@
       </c>
       <c r="H22" s="5"/>
       <c r="L22" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C23" s="4">
+        <v>30</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D23" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>43</v>
       </c>
       <c r="H23" s="5"/>
       <c r="L23" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D24" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>5</v>
@@ -1536,12 +1582,12 @@
       </c>
       <c r="H24" s="5"/>
       <c r="L24" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>5</v>
@@ -1554,12 +1600,21 @@
       </c>
       <c r="H25" s="5"/>
       <c r="L25" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C26" s="4">
+        <v>31</v>
+      </c>
       <c r="D26" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>5</v>
@@ -1572,21 +1627,21 @@
       </c>
       <c r="H26" s="5"/>
       <c r="L26" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C27" s="4">
         <v>7</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>5</v>
@@ -1599,25 +1654,23 @@
       </c>
       <c r="H27" s="5"/>
       <c r="L27" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>173</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="B29" s="8"/>
       <c r="C29" s="4">
         <v>8</v>
       </c>
@@ -1639,6 +1692,12 @@
       </c>
     </row>
     <row r="30" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C30" s="4">
+        <v>32</v>
+      </c>
       <c r="D30" s="5" t="s">
         <v>48</v>
       </c>
@@ -1678,6 +1737,12 @@
       </c>
     </row>
     <row r="32" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C32" s="4">
+        <v>33</v>
+      </c>
       <c r="D32" s="5" t="s">
         <v>50</v>
       </c>
@@ -1720,6 +1785,12 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C34" s="4">
+        <v>34</v>
+      </c>
       <c r="D34" s="5" t="s">
         <v>56</v>
       </c>
@@ -1742,16 +1813,14 @@
     </row>
     <row r="35" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>173</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="B35" s="8"/>
       <c r="C35" s="4">
         <v>9</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>40</v>
@@ -1822,6 +1891,12 @@
       </c>
     </row>
     <row r="39" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C39" s="4">
+        <v>35</v>
+      </c>
       <c r="D39" s="5" t="s">
         <v>63</v>
       </c>
@@ -1841,11 +1916,9 @@
     </row>
     <row r="40" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>173</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="B40" s="8"/>
       <c r="C40" s="4">
         <v>10</v>
       </c>
@@ -1885,6 +1958,12 @@
       </c>
     </row>
     <row r="42" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="4">
+        <v>36</v>
+      </c>
       <c r="D42" s="5" t="s">
         <v>67</v>
       </c>
@@ -1922,7 +2001,7 @@
     </row>
     <row r="44" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D44" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>40</v>
@@ -1935,12 +2014,18 @@
       </c>
       <c r="H44" s="5"/>
       <c r="L44" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" s="4">
+        <v>37</v>
+      </c>
       <c r="D45" s="5" t="s">
-        <v>72</v>
+        <v>174</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>40</v>
@@ -1953,12 +2038,12 @@
       </c>
       <c r="H45" s="5"/>
       <c r="L45" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D46" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>40</v>
@@ -1971,12 +2056,18 @@
       </c>
       <c r="H46" s="5"/>
       <c r="L46" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C47" s="4">
+        <v>38</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D47" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>40</v>
@@ -1989,21 +2080,19 @@
       </c>
       <c r="H47" s="5"/>
       <c r="L47" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>173</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="B48" s="8"/>
       <c r="C48" s="4">
         <v>11</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>40</v>
@@ -2016,12 +2105,12 @@
       </c>
       <c r="H48" s="5"/>
       <c r="L48" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D49" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>40</v>
@@ -2034,12 +2123,12 @@
       </c>
       <c r="H49" s="5"/>
       <c r="L49" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D50" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>40</v>
@@ -2052,21 +2141,19 @@
       </c>
       <c r="H50" s="5"/>
       <c r="L50" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="4">
+        <v>12</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C51" s="4">
-        <v>12</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>40</v>
@@ -2079,12 +2166,18 @@
       </c>
       <c r="H51" s="5"/>
       <c r="L51" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C52" s="4">
+        <v>39</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D52" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>40</v>
@@ -2097,21 +2190,19 @@
       </c>
       <c r="H52" s="5"/>
       <c r="L52" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>173</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="B53" s="8"/>
       <c r="C53" s="4">
         <v>13</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>40</v>
@@ -2124,12 +2215,18 @@
       </c>
       <c r="H53" s="5"/>
       <c r="L53" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C54" s="4">
+        <v>40</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D54" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>40</v>
@@ -2142,12 +2239,12 @@
       </c>
       <c r="H54" s="5"/>
       <c r="L54" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D55" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>40</v>
@@ -2160,12 +2257,18 @@
       </c>
       <c r="H55" s="5"/>
       <c r="L55" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C56" s="4">
+        <v>41</v>
+      </c>
       <c r="D56" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>40</v>
@@ -2178,12 +2281,12 @@
       </c>
       <c r="H56" s="5"/>
       <c r="L56" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D57" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>40</v>
@@ -2194,12 +2297,18 @@
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="L57" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C58" s="4">
+        <v>42</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D58" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>40</v>
@@ -2210,12 +2319,12 @@
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
       <c r="L58" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D59" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>40</v>
@@ -2226,15 +2335,21 @@
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
       <c r="L59" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R59" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C60" s="4">
+        <v>43</v>
+      </c>
       <c r="D60" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>40</v>
@@ -2245,15 +2360,15 @@
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
       <c r="L60" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="R60" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="R60" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D61" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>40</v>
@@ -2264,12 +2379,18 @@
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
       <c r="L61" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C62" s="4">
+        <v>44</v>
+      </c>
+      <c r="D62" s="5" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D62" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>40</v>
@@ -2280,12 +2401,18 @@
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
       <c r="L62" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C63" s="4">
+        <v>45</v>
+      </c>
+      <c r="D63" s="5" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D63" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>40</v>
@@ -2296,21 +2423,19 @@
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="L63" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>173</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="B64" s="8"/>
       <c r="C64" s="4">
         <v>14</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>40</v>
@@ -2323,12 +2448,18 @@
       </c>
       <c r="H64" s="5"/>
       <c r="L64" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C65" s="4">
+        <v>46</v>
+      </c>
       <c r="D65" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>40</v>
@@ -2339,89 +2470,89 @@
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="L65" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
     </row>
-    <row r="67" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C67" s="4">
         <v>15</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H67" s="5"/>
       <c r="L67" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C68" s="4">
         <v>16</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L68" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C69" s="4">
         <v>17</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>6</v>
@@ -2431,27 +2562,27 @@
       </c>
       <c r="H69" s="5"/>
       <c r="L69" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="R69" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="R69" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C70" s="4">
         <v>18</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>15</v>
@@ -2460,81 +2591,92 @@
         <v>18</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L70" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C71" s="4">
+        <v>47</v>
+      </c>
       <c r="D71" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="E71" s="5"/>
+        <v>147</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>137</v>
+      </c>
       <c r="F71" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L71" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C72" s="4">
         <v>19</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G72" s="5"/>
       <c r="H72" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L72" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C73" s="4">
         <v>20</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>6</v>
@@ -2544,24 +2686,24 @@
       </c>
       <c r="H73" s="5"/>
       <c r="L73" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C74" s="4">
         <v>21</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>6</v>
@@ -2571,47 +2713,56 @@
       </c>
       <c r="H74" s="5"/>
       <c r="L74" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="75" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C75" s="4">
+        <v>48</v>
+      </c>
       <c r="D75" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L75" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C76" s="4">
         <v>22</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>15</v>
@@ -2620,53 +2771,59 @@
         <v>18</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L76" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="77" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C77" s="4">
         <v>23</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L77" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C78" s="4">
+        <v>49</v>
+      </c>
       <c r="D78" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>8</v>
@@ -2676,57 +2833,57 @@
       </c>
       <c r="H78" s="5"/>
       <c r="L78" s="6" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C79" s="4">
         <v>24</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G79" s="5"/>
       <c r="H79" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L79" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C80" s="4">
         <v>25</v>
       </c>
       <c r="D80" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E80" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>15</v>
@@ -2735,10 +2892,10 @@
         <v>18</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L80" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="81" spans="2:8" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -3033,11 +3190,11 @@
       <c r="B1048517" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V81">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="40-60"/>
-      </filters>
+  <autoFilter ref="A1:V81" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
     <filterColumn colId="6" showButton="0"/>
     <filterColumn colId="7" showButton="0"/>

</xml_diff>

<commit_message>
add back btn to workout form
</commit_message>
<xml_diff>
--- a/ocr-workouts/workouts.xlsx
+++ b/ocr-workouts/workouts.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamkuhn/workspace/bootcamp/workout-generator/ocr-workouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C8E6441C-FD1B-7B4F-8F22-91F095386AB2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B2EA707E-3191-984C-BB17-5C25F556C1F1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="460" windowWidth="21500" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7980" yWindow="1780" windowWidth="21500" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OCR Workouts" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OCR Workouts'!$A$1:$V$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OCR Workouts'!$A$1:$V$80</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="175">
   <si>
     <t>ID</t>
   </si>
@@ -394,9 +394,6 @@
   </si>
   <si>
     <t>10 min warm up, 50 min AMRAP: 100 m hill sprint, sandbag/bucket carry up the hill, 10 pull ups, 10 push ups, 100 m hill sprint, 10 sandbag/bucket squats, 250 m race pace run, 10 box jumps (or squat jumps), 15 burpees. Finisher: 3x 10 toes2bar - deadhang to failure - 2 min plank</t>
-  </si>
-  <si>
-    <t>Add 10 strength workout with varying equipment, same with OCR wods</t>
   </si>
   <si>
     <t>JayMan</t>
@@ -1006,11 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:R1048517"/>
+  <dimension ref="A1:R1048516"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1029,10 +1025,10 @@
   <sheetData>
     <row r="1" spans="1:18" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1067,10 +1063,10 @@
     </row>
     <row r="2" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -1085,14 +1081,14 @@
         <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H2" s="5"/>
       <c r="L2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="5" t="s">
         <v>26</v>
       </c>
@@ -1110,7 +1106,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="5" t="s">
         <v>27</v>
       </c>
@@ -1130,10 +1126,10 @@
     </row>
     <row r="5" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C5" s="4">
         <v>2</v>
@@ -1155,7 +1151,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="5" t="s">
         <v>29</v>
       </c>
@@ -1173,7 +1169,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1191,7 +1187,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="5" t="s">
         <v>31</v>
       </c>
@@ -1211,10 +1207,10 @@
     </row>
     <row r="9" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C9" s="4">
         <v>26</v>
@@ -1238,10 +1234,10 @@
     </row>
     <row r="10" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C10" s="4">
         <v>3</v>
@@ -1265,10 +1261,10 @@
     </row>
     <row r="11" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C11" s="4">
         <v>27</v>
@@ -1290,7 +1286,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D12" s="5" t="s">
         <v>25</v>
       </c>
@@ -1308,7 +1304,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" s="5" t="s">
         <v>20</v>
       </c>
@@ -1328,10 +1324,10 @@
     </row>
     <row r="14" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C14" s="4">
         <v>4</v>
@@ -1355,10 +1351,10 @@
     </row>
     <row r="15" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C15" s="8">
         <v>28</v>
@@ -1380,7 +1376,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D16" s="5" t="s">
         <v>22</v>
       </c>
@@ -1400,10 +1396,10 @@
     </row>
     <row r="17" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C17" s="4">
         <v>5</v>
@@ -1429,10 +1425,10 @@
     </row>
     <row r="18" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C18" s="4">
         <v>29</v>
@@ -1454,7 +1450,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D19" s="5" t="s">
         <v>39</v>
       </c>
@@ -1474,10 +1470,10 @@
     </row>
     <row r="20" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C20" s="4">
         <v>6</v>
@@ -1502,7 +1498,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" s="5" t="s">
         <v>119</v>
       </c>
@@ -1522,9 +1518,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D22" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>5</v>
@@ -1537,21 +1533,21 @@
       </c>
       <c r="H22" s="5"/>
       <c r="L22" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C23" s="4">
         <v>30</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>5</v>
@@ -1564,12 +1560,12 @@
       </c>
       <c r="H23" s="5"/>
       <c r="L23" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D24" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>5</v>
@@ -1582,12 +1578,12 @@
       </c>
       <c r="H24" s="5"/>
       <c r="L24" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>5</v>
@@ -1600,21 +1596,21 @@
       </c>
       <c r="H25" s="5"/>
       <c r="L25" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C26" s="4">
         <v>31</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>5</v>
@@ -1627,21 +1623,21 @@
       </c>
       <c r="H26" s="5"/>
       <c r="L26" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C27" s="4">
         <v>7</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>5</v>
@@ -1654,10 +1650,10 @@
       </c>
       <c r="H27" s="5"/>
       <c r="L27" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
         <v>89</v>
@@ -1668,7 +1664,7 @@
     </row>
     <row r="29" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="4">
@@ -1693,7 +1689,7 @@
     </row>
     <row r="30" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C30" s="4">
         <v>32</v>
@@ -1715,7 +1711,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D31" s="5" t="s">
         <v>49</v>
       </c>
@@ -1738,7 +1734,7 @@
     </row>
     <row r="32" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C32" s="4">
         <v>33</v>
@@ -1763,7 +1759,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D33" s="5" t="s">
         <v>55</v>
       </c>
@@ -1786,7 +1782,7 @@
     </row>
     <row r="34" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C34" s="4">
         <v>34</v>
@@ -1813,14 +1809,14 @@
     </row>
     <row r="35" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="4">
         <v>9</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>40</v>
@@ -1836,7 +1832,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D36" s="5" t="s">
         <v>57</v>
       </c>
@@ -1854,7 +1850,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D37" s="5" t="s">
         <v>58</v>
       </c>
@@ -1872,7 +1868,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D38" s="5" t="s">
         <v>61</v>
       </c>
@@ -1892,7 +1888,7 @@
     </row>
     <row r="39" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C39" s="4">
         <v>35</v>
@@ -1916,7 +1912,7 @@
     </row>
     <row r="40" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="4">
@@ -1939,7 +1935,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D41" s="5" t="s">
         <v>70</v>
       </c>
@@ -1959,7 +1955,7 @@
     </row>
     <row r="42" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C42" s="4">
         <v>36</v>
@@ -1981,7 +1977,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D43" s="5" t="s">
         <v>67</v>
       </c>
@@ -1999,7 +1995,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D44" s="5" t="s">
         <v>72</v>
       </c>
@@ -2019,13 +2015,13 @@
     </row>
     <row r="45" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C45" s="4">
         <v>37</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>40</v>
@@ -2041,7 +2037,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D46" s="5" t="s">
         <v>77</v>
       </c>
@@ -2061,7 +2057,7 @@
     </row>
     <row r="47" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C47" s="4">
         <v>38</v>
@@ -2085,7 +2081,7 @@
     </row>
     <row r="48" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="4">
@@ -2108,7 +2104,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D49" s="5" t="s">
         <v>81</v>
       </c>
@@ -2126,7 +2122,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D50" s="5" t="s">
         <v>83</v>
       </c>
@@ -2146,7 +2142,7 @@
     </row>
     <row r="51" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="4">
@@ -2171,7 +2167,7 @@
     </row>
     <row r="52" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C52" s="4">
         <v>39</v>
@@ -2195,7 +2191,7 @@
     </row>
     <row r="53" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="4">
@@ -2220,7 +2216,7 @@
     </row>
     <row r="54" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C54" s="4">
         <v>40</v>
@@ -2242,7 +2238,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D55" s="5" t="s">
         <v>95</v>
       </c>
@@ -2262,7 +2258,7 @@
     </row>
     <row r="56" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C56" s="4">
         <v>41</v>
@@ -2284,7 +2280,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D57" s="5" t="s">
         <v>98</v>
       </c>
@@ -2302,7 +2298,7 @@
     </row>
     <row r="58" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C58" s="4">
         <v>42</v>
@@ -2322,7 +2318,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D59" s="5" t="s">
         <v>105</v>
       </c>
@@ -2343,7 +2339,7 @@
     </row>
     <row r="60" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C60" s="4">
         <v>43</v>
@@ -2366,7 +2362,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D61" s="5" t="s">
         <v>107</v>
       </c>
@@ -2384,7 +2380,7 @@
     </row>
     <row r="62" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C62" s="4">
         <v>44</v>
@@ -2406,7 +2402,7 @@
     </row>
     <row r="63" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C63" s="4">
         <v>45</v>
@@ -2428,14 +2424,14 @@
     </row>
     <row r="64" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="4">
         <v>14</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>40</v>
@@ -2453,7 +2449,7 @@
     </row>
     <row r="65" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C65" s="4">
         <v>46</v>
@@ -2473,210 +2469,228 @@
         <v>115</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D66" s="5"/>
+    <row r="66" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C66" s="4">
+        <v>15</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="E66" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
+        <v>136</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>152</v>
+      </c>
       <c r="H66" s="5"/>
+      <c r="L66" s="6" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="67" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C67" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="H67" s="5"/>
+        <v>134</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>133</v>
+      </c>
       <c r="L67" s="6" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C68" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>134</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H68" s="5"/>
       <c r="L68" s="6" t="s">
-        <v>132</v>
+        <v>143</v>
+      </c>
+      <c r="R68" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C69" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H69" s="5"/>
+      <c r="H69" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>147</v>
+      </c>
       <c r="L69" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="R69" s="4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C70" s="4">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>18</v>
+        <v>134</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L70" s="6" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C71" s="4">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G71" s="5" t="s">
-        <v>135</v>
-      </c>
+      <c r="G71" s="5"/>
       <c r="H71" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="I71" s="4" t="s">
-        <v>148</v>
+        <v>133</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="L71" s="6" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C72" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H72" s="5"/>
       <c r="L72" s="6" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C73" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>6</v>
@@ -2686,325 +2700,308 @@
       </c>
       <c r="H73" s="5"/>
       <c r="L73" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="74" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C74" s="4">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H74" s="5"/>
+        <v>134</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L74" s="6" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="75" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C75" s="4">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>135</v>
+        <v>18</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="J75" s="4" t="s">
-        <v>18</v>
+        <v>133</v>
       </c>
       <c r="L75" s="6" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C76" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G76" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J76" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H76" s="5" t="s">
-        <v>134</v>
-      </c>
       <c r="L76" s="6" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C77" s="4">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="I77" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J77" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="H77" s="5"/>
       <c r="L77" s="6" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>170</v>
       </c>
       <c r="C78" s="4">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G78" s="5" t="s">
+      <c r="G78" s="5"/>
+      <c r="H78" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J78" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H78" s="5"/>
       <c r="L78" s="6" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C79" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G79" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="H79" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="I79" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J79" s="4" t="s">
-        <v>18</v>
+        <v>133</v>
       </c>
       <c r="L79" s="6" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C80" s="4">
-        <v>25</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H80" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="L80" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="81" spans="2:8" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="8"/>
+      <c r="B80" s="8"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
     </row>
-    <row r="82" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
     </row>
-    <row r="83" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
     </row>
-    <row r="84" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
     </row>
-    <row r="85" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
       <c r="H85" s="5"/>
     </row>
-    <row r="86" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
     </row>
-    <row r="87" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
       <c r="H87" s="5"/>
     </row>
-    <row r="88" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
       <c r="G88" s="5"/>
       <c r="H88" s="5"/>
     </row>
-    <row r="89" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
     </row>
-    <row r="90" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
     </row>
-    <row r="91" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
     </row>
-    <row r="92" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
     </row>
-    <row r="93" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
       <c r="H93" s="5"/>
     </row>
-    <row r="94" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
       <c r="G94" s="5"/>
       <c r="H94" s="5"/>
     </row>
-    <row r="95" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
       <c r="G95" s="5"/>
       <c r="H95" s="5"/>
     </row>
-    <row r="96" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
@@ -3179,23 +3176,11 @@
       <c r="G120" s="5"/>
       <c r="H120" s="5"/>
     </row>
-    <row r="121" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
-      <c r="G121" s="5"/>
-      <c r="H121" s="5"/>
-    </row>
-    <row r="1048517" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1048517" s="7"/>
+    <row r="1048516" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1048516" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V81" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
+  <autoFilter ref="A1:V80" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="6" showButton="0"/>
     <filterColumn colId="7" showButton="0"/>
     <filterColumn colId="8" showButton="0"/>

</xml_diff>

<commit_message>
server ind var to const
</commit_message>
<xml_diff>
--- a/ocr-workouts/workouts.xlsx
+++ b/ocr-workouts/workouts.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamkuhn/workspace/bootcamp/workout-generator/ocr-workouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{871C500C-1DF8-9E4E-A8EC-E4DAAA3FCB98}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E745191C-DBC1-5645-8570-2F6686FA3C6B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="580" windowWidth="21500" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12620" yWindow="2440" windowWidth="21500" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OCR Workouts" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OCR Workouts'!$A$1:$V$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OCR Workouts'!$A$1:$V$83</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="181">
   <si>
     <t>ID</t>
   </si>
@@ -297,9 +297,6 @@
     <t>10 min warm up, 5x 1000 m repeats, rest 2:00-2:30, 10 min cool down</t>
   </si>
   <si>
-    <t>insert tempo ocr with pushups etc</t>
-  </si>
-  <si>
     <t>Fartleking</t>
   </si>
   <si>
@@ -553,6 +550,27 @@
   </si>
   <si>
     <t>Long Fartlek</t>
+  </si>
+  <si>
+    <t>Spartan KB</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>5 rounds: 200 m run, 2x KB clean and press (each side), 5x Goblet Squat, 20x kb swings, rest 2 min</t>
+  </si>
+  <si>
+    <t>One Arm Swing</t>
+  </si>
+  <si>
+    <t>10 rounds: 30s one armed KB swing (left), 30s rest, 30s one armed KB swing (right, 30s rest)</t>
+  </si>
+  <si>
+    <t>Farmer Squat</t>
+  </si>
+  <si>
+    <t>5 rounds: suit case carry 20 m (left hand) - 1 x front squat - 20 m carry (left hand) - 2x front squat - 20 m carry - 3x front squat, repeat with right arm. 1 round = left and right arm</t>
   </si>
 </sst>
 </file>
@@ -637,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -657,6 +675,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1034,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R1048517"/>
+  <dimension ref="A1:R1048519"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1056,10 +1084,10 @@
   <sheetData>
     <row r="1" spans="1:18" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1094,10 +1122,10 @@
     </row>
     <row r="2" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -1112,7 +1140,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H2" s="5"/>
       <c r="L2" s="6" t="s">
@@ -1121,10 +1149,10 @@
     </row>
     <row r="3" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C3" s="4">
         <v>52</v>
@@ -1148,10 +1176,10 @@
     </row>
     <row r="4" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C4" s="4">
         <v>53</v>
@@ -1175,10 +1203,10 @@
     </row>
     <row r="5" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C5" s="4">
         <v>2</v>
@@ -1202,7 +1230,7 @@
     </row>
     <row r="6" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" s="4">
         <v>67</v>
@@ -1226,10 +1254,10 @@
     </row>
     <row r="7" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C7" s="4">
         <v>50</v>
@@ -1253,10 +1281,10 @@
     </row>
     <row r="8" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C8" s="8">
         <v>54</v>
@@ -1280,10 +1308,10 @@
     </row>
     <row r="9" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C9" s="4">
         <v>26</v>
@@ -1307,10 +1335,10 @@
     </row>
     <row r="10" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C10" s="4">
         <v>3</v>
@@ -1334,10 +1362,10 @@
     </row>
     <row r="11" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C11" s="4">
         <v>27</v>
@@ -1361,10 +1389,10 @@
     </row>
     <row r="12" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C12" s="4">
         <v>68</v>
@@ -1388,10 +1416,10 @@
     </row>
     <row r="13" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C13" s="4">
         <v>51</v>
@@ -1415,10 +1443,10 @@
     </row>
     <row r="14" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C14" s="4">
         <v>4</v>
@@ -1442,10 +1470,10 @@
     </row>
     <row r="15" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C15" s="8">
         <v>28</v>
@@ -1469,10 +1497,10 @@
     </row>
     <row r="16" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C16" s="8">
         <v>69</v>
@@ -1496,16 +1524,16 @@
     </row>
     <row r="17" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C17" s="4">
         <v>5</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>5</v>
@@ -1517,18 +1545,18 @@
         <v>18</v>
       </c>
       <c r="H17" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C18" s="4">
         <v>29</v>
@@ -1552,10 +1580,10 @@
     </row>
     <row r="19" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C19" s="8">
         <v>70</v>
@@ -1579,10 +1607,10 @@
     </row>
     <row r="20" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C20" s="4">
         <v>6</v>
@@ -1609,77 +1637,77 @@
     </row>
     <row r="21" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C21" s="8">
         <v>71</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C22" s="8">
         <v>72</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>18</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C23" s="4">
         <v>55</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>5</v>
@@ -1692,21 +1720,21 @@
       </c>
       <c r="H23" s="5"/>
       <c r="L23" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C24" s="4">
         <v>30</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>5</v>
@@ -1719,21 +1747,21 @@
       </c>
       <c r="H24" s="5"/>
       <c r="L24" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C25" s="4">
         <v>73</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>5</v>
@@ -1746,21 +1774,21 @@
       </c>
       <c r="H25" s="5"/>
       <c r="L25" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C26" s="4">
         <v>56</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>5</v>
@@ -1773,21 +1801,21 @@
       </c>
       <c r="H26" s="5"/>
       <c r="L26" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C27" s="4">
         <v>31</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>5</v>
@@ -1800,21 +1828,21 @@
       </c>
       <c r="H27" s="5"/>
       <c r="L27" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C28" s="4">
         <v>7</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>5</v>
@@ -1827,76 +1855,103 @@
       </c>
       <c r="H28" s="5"/>
       <c r="L28" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D29" s="5"/>
+      <c r="A29" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="4">
+        <v>79</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>174</v>
+      </c>
       <c r="E29" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>175</v>
+      </c>
       <c r="H29" s="5"/>
+      <c r="L29" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
     </row>
     <row r="30" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="4">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>47</v>
+        <v>179</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="5"/>
+        <v>175</v>
+      </c>
+      <c r="H30" s="13"/>
       <c r="L30" s="6" t="s">
-        <v>41</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="M30" s="11"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
     </row>
     <row r="31" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C31" s="4">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>48</v>
+        <v>177</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>12</v>
+        <v>175</v>
       </c>
       <c r="H31" s="5"/>
       <c r="L31" s="6" t="s">
-        <v>42</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>169</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="B32" s="8"/>
       <c r="C32" s="4">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>40</v>
@@ -1909,21 +1964,18 @@
       </c>
       <c r="H32" s="5"/>
       <c r="L32" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="R32" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C33" s="4">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>40</v>
@@ -1936,21 +1988,18 @@
       </c>
       <c r="H33" s="5"/>
       <c r="L33" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="R33" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C34" s="4">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>40</v>
@@ -1963,21 +2012,21 @@
       </c>
       <c r="H34" s="5"/>
       <c r="L34" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="R34" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C35" s="4">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>40</v>
@@ -1990,94 +2039,100 @@
       </c>
       <c r="H35" s="5"/>
       <c r="L35" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B36" s="8"/>
+        <v>168</v>
+      </c>
       <c r="C36" s="4">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>162</v>
+        <v>55</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H36" s="5"/>
       <c r="L36" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="R36" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C37" s="4">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H37" s="5"/>
       <c r="L37" s="6" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="R37" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>169</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="B38" s="8"/>
       <c r="C38" s="4">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>58</v>
+        <v>161</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H38" s="5"/>
       <c r="L38" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C39" s="4">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>40</v>
@@ -2090,91 +2145,91 @@
       </c>
       <c r="H39" s="5"/>
       <c r="L39" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C40" s="4">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H40" s="5"/>
       <c r="L40" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B41" s="8"/>
+        <v>168</v>
+      </c>
       <c r="C41" s="4">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H41" s="5"/>
       <c r="L41" s="6" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C42" s="4">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H42" s="5"/>
       <c r="L42" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>169</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="B43" s="8"/>
       <c r="C43" s="4">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>40</v>
@@ -2187,18 +2242,18 @@
       </c>
       <c r="H43" s="5"/>
       <c r="L43" s="6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C44" s="4">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>40</v>
@@ -2211,66 +2266,66 @@
       </c>
       <c r="H44" s="5"/>
       <c r="L44" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C45" s="4">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H45" s="5"/>
       <c r="L45" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C46" s="4">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>172</v>
+        <v>67</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H46" s="5"/>
       <c r="L46" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C47" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>40</v>
@@ -2283,18 +2338,18 @@
       </c>
       <c r="H47" s="5"/>
       <c r="L47" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C48" s="4">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>40</v>
@@ -2307,141 +2362,140 @@
       </c>
       <c r="H48" s="5"/>
       <c r="L48" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B49" s="8"/>
+        <v>168</v>
+      </c>
       <c r="C49" s="4">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H49" s="5"/>
       <c r="L49" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C50" s="4">
+        <v>38</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="E50" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H50" s="5"/>
       <c r="L50" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>169</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="B51" s="8"/>
       <c r="C51" s="4">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H51" s="5"/>
       <c r="L51" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B52" s="8"/>
+        <v>168</v>
+      </c>
       <c r="C52" s="4">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H52" s="5"/>
       <c r="L52" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C53" s="4">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H53" s="5"/>
       <c r="L53" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>40</v>
@@ -2450,22 +2504,22 @@
         <v>6</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H54" s="5"/>
       <c r="L54" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C55" s="4">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>40</v>
@@ -2474,46 +2528,47 @@
         <v>8</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H55" s="5"/>
       <c r="L55" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>169</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="B56" s="8"/>
       <c r="C56" s="4">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>174</v>
+        <v>89</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>43</v>
       </c>
       <c r="H56" s="5"/>
       <c r="L56" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C57" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>40</v>
@@ -2526,40 +2581,42 @@
       </c>
       <c r="H57" s="5"/>
       <c r="L57" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C58" s="4">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>97</v>
+        <v>173</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G58" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="H58" s="5"/>
       <c r="L58" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C59" s="4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>40</v>
@@ -2567,21 +2624,23 @@
       <c r="F59" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G59" s="5"/>
+      <c r="G59" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="H59" s="5"/>
       <c r="L59" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C60" s="4">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>40</v>
@@ -2592,21 +2651,18 @@
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
       <c r="L60" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="R60" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C61" s="4">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>40</v>
@@ -2617,21 +2673,18 @@
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
       <c r="L61" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="R61" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C62" s="4">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>40</v>
@@ -2642,18 +2695,21 @@
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
       <c r="L62" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
+      </c>
+      <c r="R62" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C63" s="4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>40</v>
@@ -2664,65 +2720,65 @@
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="L63" s="6" t="s">
-        <v>109</v>
+        <v>101</v>
+      </c>
+      <c r="R63" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="64" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C64" s="4">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="L64" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B65" s="8"/>
+        <v>168</v>
+      </c>
       <c r="C65" s="4">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G65" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="L65" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C66" s="4">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>40</v>
@@ -2733,535 +2789,568 @@
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
       <c r="L66" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>169</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="B67" s="8"/>
       <c r="C67" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>127</v>
+        <v>162</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>151</v>
+        <v>43</v>
       </c>
       <c r="H67" s="5"/>
       <c r="L67" s="6" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
     </row>
     <row r="68" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C68" s="4">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
       <c r="L68" s="6" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C69" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>18</v>
+        <v>150</v>
       </c>
       <c r="H69" s="5"/>
       <c r="L69" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="R69" s="4" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C70" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="I70" s="4" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="L70" s="6" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C71" s="4">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="H71" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="I71" s="4" t="s">
-        <v>146</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H71" s="5"/>
       <c r="L71" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
+      </c>
+      <c r="R71" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C72" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G72" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="H72" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>18</v>
+        <v>131</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="L72" s="6" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C73" s="4">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H73" s="5"/>
+        <v>132</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>145</v>
+      </c>
       <c r="L73" s="6" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C74" s="4">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H74" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L74" s="6" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C75" s="4">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="J75" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H75" s="5"/>
       <c r="L75" s="6" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C76" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>132</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H76" s="5"/>
       <c r="L76" s="6" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
     </row>
     <row r="77" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C77" s="4">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="I77" s="4" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L77" s="6" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C78" s="4">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H78" s="5"/>
+      <c r="H78" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="L78" s="6" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C79" s="4">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G79" s="5"/>
+      <c r="G79" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="H79" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L79" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="80" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C80" s="4">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D80" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E80" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E80" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="F80" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H80" s="5" t="s">
-        <v>132</v>
-      </c>
+      <c r="H80" s="5"/>
       <c r="L80" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C81" s="4">
+        <v>24</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="81" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="8"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
-    </row>
-    <row r="82" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="5"/>
-      <c r="H82" s="5"/>
-    </row>
-    <row r="83" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I81" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L81" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" s="4">
+        <v>25</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="L82" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B83" s="8"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
     </row>
-    <row r="84" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
     </row>
-    <row r="85" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
       <c r="H85" s="5"/>
     </row>
-    <row r="86" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
     </row>
-    <row r="87" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
       <c r="H87" s="5"/>
     </row>
-    <row r="88" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
       <c r="G88" s="5"/>
       <c r="H88" s="5"/>
     </row>
-    <row r="89" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
     </row>
-    <row r="90" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
     </row>
-    <row r="91" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
     </row>
-    <row r="92" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
     </row>
-    <row r="93" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
       <c r="H93" s="5"/>
     </row>
-    <row r="94" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
       <c r="G94" s="5"/>
       <c r="H94" s="5"/>
     </row>
-    <row r="95" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
       <c r="G95" s="5"/>
       <c r="H95" s="5"/>
     </row>
-    <row r="96" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
@@ -3443,11 +3532,25 @@
       <c r="G121" s="5"/>
       <c r="H121" s="5"/>
     </row>
-    <row r="1048517" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1048517" s="7"/>
+    <row r="122" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D122" s="5"/>
+      <c r="E122" s="5"/>
+      <c r="F122" s="5"/>
+      <c r="G122" s="5"/>
+      <c r="H122" s="5"/>
+    </row>
+    <row r="123" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D123" s="5"/>
+      <c r="E123" s="5"/>
+      <c r="F123" s="5"/>
+      <c r="G123" s="5"/>
+      <c r="H123" s="5"/>
+    </row>
+    <row r="1048519" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1048519" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V81" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:V83" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="6" showButton="0"/>
     <filterColumn colId="7" showButton="0"/>
     <filterColumn colId="8" showButton="0"/>
@@ -3458,9 +3561,10 @@
     <filterColumn colId="14" showButton="0"/>
     <filterColumn colId="15" showButton="0"/>
   </autoFilter>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="L29:Q29"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:B20 A22:B1048576">
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="YES">

</xml_diff>

<commit_message>
set up basic waiting
</commit_message>
<xml_diff>
--- a/ocr-workouts/workouts.xlsx
+++ b/ocr-workouts/workouts.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamkuhn/workspace/bootcamp/workout-generator/ocr-workouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E745191C-DBC1-5645-8570-2F6686FA3C6B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3A3C4F3A-E928-2046-89E0-BB80AFEF1566}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12620" yWindow="2440" windowWidth="21500" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4100" yWindow="2640" windowWidth="21500" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OCR Workouts" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OCR Workouts'!$A$1:$V$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OCR Workouts'!$A$2:$V$84</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="184">
   <si>
     <t>ID</t>
   </si>
@@ -571,6 +571,15 @@
   </si>
   <si>
     <t>5 rounds: suit case carry 20 m (left hand) - 1 x front squat - 20 m carry (left hand) - 2x front squat - 20 m carry - 3x front squat, repeat with right arm. 1 round = left and right arm</t>
+  </si>
+  <si>
+    <t>NOTE: When updating live APP must rollback migrations in Bash (knex migrate:rollback), then knex migrate:latest, then knex seed:run</t>
+  </si>
+  <si>
+    <t>Gasses</t>
+  </si>
+  <si>
+    <t>3-5 rounds: 10 thrusters (95 lb), ~100 m sprint, 10 pull ups, 100 m sprint, rest</t>
   </si>
 </sst>
 </file>
@@ -655,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -669,12 +678,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -685,6 +688,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1062,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R1048519"/>
+  <dimension ref="A1:R1048520"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="L84" sqref="L84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1082,69 +1094,53 @@
     <col min="19" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10" t="s">
-        <v>10</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="L1" s="10"/>
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
       <c r="O1" s="10"/>
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
-      <c r="R1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:18" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="3" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="L2" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1155,10 +1151,10 @@
         <v>168</v>
       </c>
       <c r="C3" s="4">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>5</v>
@@ -1167,11 +1163,11 @@
         <v>6</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="H3" s="5"/>
       <c r="L3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1182,10 +1178,10 @@
         <v>168</v>
       </c>
       <c r="C4" s="4">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>5</v>
@@ -1198,7 +1194,7 @@
       </c>
       <c r="H4" s="5"/>
       <c r="L4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1209,16 +1205,16 @@
         <v>168</v>
       </c>
       <c r="C5" s="4">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>12</v>
@@ -1232,17 +1228,20 @@
       <c r="A6" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>168</v>
+      </c>
       <c r="C6" s="4">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>12</v>
@@ -1256,47 +1255,44 @@
       <c r="A7" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>168</v>
-      </c>
       <c r="C7" s="4">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="5"/>
       <c r="L7" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="8">
-        <v>54</v>
+      <c r="B8" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="4">
+        <v>50</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>12</v>
@@ -1310,20 +1306,20 @@
       <c r="A9" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C9" s="4">
-        <v>26</v>
+      <c r="B9" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="8">
+        <v>54</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>12</v>
@@ -1341,16 +1337,16 @@
         <v>168</v>
       </c>
       <c r="C10" s="4">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>12</v>
@@ -1364,47 +1360,47 @@
       <c r="A11" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="4" t="s">
         <v>168</v>
       </c>
       <c r="C11" s="4">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="5"/>
       <c r="L11" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="8" t="s">
         <v>168</v>
       </c>
       <c r="C12" s="4">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>12</v>
@@ -1422,43 +1418,43 @@
         <v>168</v>
       </c>
       <c r="C13" s="4">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H13" s="5"/>
       <c r="L13" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="4" t="s">
         <v>168</v>
       </c>
       <c r="C14" s="4">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>18</v>
@@ -1475,17 +1471,17 @@
       <c r="B15" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C15" s="8">
-        <v>28</v>
+      <c r="C15" s="4">
+        <v>4</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>18</v>
@@ -1503,16 +1499,16 @@
         <v>168</v>
       </c>
       <c r="C16" s="8">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>18</v>
@@ -1529,26 +1525,24 @@
       <c r="B17" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C17" s="4">
-        <v>5</v>
+      <c r="C17" s="8">
+        <v>69</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>114</v>
+        <v>22</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>115</v>
-      </c>
+      <c r="H17" s="5"/>
       <c r="L17" s="6" t="s">
-        <v>116</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1559,10 +1553,10 @@
         <v>168</v>
       </c>
       <c r="C18" s="4">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>5</v>
@@ -1573,9 +1567,11 @@
       <c r="G18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="L18" s="6" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1585,17 +1581,17 @@
       <c r="B19" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C19" s="8">
-        <v>70</v>
+      <c r="C19" s="4">
+        <v>29</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>18</v>
@@ -1612,17 +1608,17 @@
       <c r="B20" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C20" s="4">
-        <v>6</v>
+      <c r="C20" s="8">
+        <v>70</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>18</v>
@@ -1631,9 +1627,6 @@
       <c r="L20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="R20" s="4" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="21" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
@@ -1642,26 +1635,27 @@
       <c r="B21" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C21" s="8">
-        <v>71</v>
+      <c r="C21" s="4">
+        <v>6</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>117</v>
+        <v>37</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>118</v>
+        <v>6</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>115</v>
-      </c>
+      <c r="H21" s="5"/>
       <c r="L21" s="6" t="s">
-        <v>119</v>
+        <v>34</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1672,7 +1666,7 @@
         <v>168</v>
       </c>
       <c r="C22" s="8">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>117</v>
@@ -1689,9 +1683,6 @@
       <c r="H22" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>145</v>
-      </c>
       <c r="L22" s="6" t="s">
         <v>119</v>
       </c>
@@ -1703,24 +1694,29 @@
       <c r="B23" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C23" s="4">
-        <v>55</v>
+      <c r="C23" s="8">
+        <v>72</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H23" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>145</v>
+      </c>
       <c r="L23" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1731,23 +1727,23 @@
         <v>168</v>
       </c>
       <c r="C24" s="4">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>43</v>
       </c>
       <c r="H24" s="5"/>
       <c r="L24" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1758,10 +1754,10 @@
         <v>168</v>
       </c>
       <c r="C25" s="4">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>5</v>
@@ -1774,7 +1770,7 @@
       </c>
       <c r="H25" s="5"/>
       <c r="L25" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1785,23 +1781,23 @@
         <v>168</v>
       </c>
       <c r="C26" s="4">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>43</v>
       </c>
       <c r="H26" s="5"/>
       <c r="L26" s="6" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1812,23 +1808,23 @@
         <v>168</v>
       </c>
       <c r="C27" s="4">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="H27" s="5"/>
       <c r="L27" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1839,10 +1835,10 @@
         <v>168</v>
       </c>
       <c r="C28" s="4">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>5</v>
@@ -1855,38 +1851,35 @@
       </c>
       <c r="H28" s="5"/>
       <c r="L28" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B29" s="8"/>
+      <c r="B29" s="8" t="s">
+        <v>168</v>
+      </c>
       <c r="C29" s="4">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>174</v>
+        <v>138</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>175</v>
+        <v>18</v>
       </c>
       <c r="H29" s="5"/>
-      <c r="L29" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
+      <c r="L29" s="6" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="30" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
@@ -1894,10 +1887,10 @@
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="4">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>5</v>
@@ -1908,25 +1901,26 @@
       <c r="G30" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="H30" s="13"/>
-      <c r="L30" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="M30" s="11"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
+      <c r="H30" s="5"/>
+      <c r="L30" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
     </row>
     <row r="31" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="B31" s="8"/>
       <c r="C31" s="4">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>5</v>
@@ -1937,58 +1931,63 @@
       <c r="G31" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="H31" s="5"/>
+      <c r="H31" s="11"/>
       <c r="L31" s="6" t="s">
-        <v>178</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="M31" s="9"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
     </row>
     <row r="32" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B32" s="8"/>
       <c r="C32" s="4">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>47</v>
+        <v>177</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>12</v>
+        <v>175</v>
       </c>
       <c r="H32" s="5"/>
       <c r="L32" s="6" t="s">
-        <v>41</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="B33" s="8"/>
       <c r="C33" s="4">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H33" s="5"/>
       <c r="L33" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1996,26 +1995,23 @@
         <v>168</v>
       </c>
       <c r="C34" s="4">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H34" s="5"/>
       <c r="L34" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="R34" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2023,23 +2019,23 @@
         <v>168</v>
       </c>
       <c r="C35" s="4">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H35" s="5"/>
       <c r="L35" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>46</v>
@@ -2050,26 +2046,26 @@
         <v>168</v>
       </c>
       <c r="C36" s="4">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H36" s="5"/>
       <c r="L36" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="R36" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2077,23 +2073,23 @@
         <v>168</v>
       </c>
       <c r="C37" s="4">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H37" s="5"/>
       <c r="L37" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>53</v>
@@ -2103,12 +2099,11 @@
       <c r="A38" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B38" s="8"/>
       <c r="C38" s="4">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>161</v>
+        <v>56</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>40</v>
@@ -2121,31 +2116,35 @@
       </c>
       <c r="H38" s="5"/>
       <c r="L38" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="R38" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="B39" s="8"/>
       <c r="C39" s="4">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H39" s="5"/>
       <c r="L39" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2153,10 +2152,10 @@
         <v>168</v>
       </c>
       <c r="C40" s="4">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>40</v>
@@ -2169,7 +2168,7 @@
       </c>
       <c r="H40" s="5"/>
       <c r="L40" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2177,10 +2176,10 @@
         <v>168</v>
       </c>
       <c r="C41" s="4">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>40</v>
@@ -2193,7 +2192,7 @@
       </c>
       <c r="H41" s="5"/>
       <c r="L41" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2201,35 +2200,34 @@
         <v>168</v>
       </c>
       <c r="C42" s="4">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H42" s="5"/>
       <c r="L42" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B43" s="8"/>
       <c r="C43" s="4">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>40</v>
@@ -2242,31 +2240,32 @@
       </c>
       <c r="H43" s="5"/>
       <c r="L43" s="6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="B44" s="8"/>
       <c r="C44" s="4">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H44" s="5"/>
       <c r="L44" s="6" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2274,23 +2273,23 @@
         <v>168</v>
       </c>
       <c r="C45" s="4">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H45" s="5"/>
       <c r="L45" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2298,7 +2297,7 @@
         <v>168</v>
       </c>
       <c r="C46" s="4">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>67</v>
@@ -2307,14 +2306,14 @@
         <v>40</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H46" s="5"/>
       <c r="L46" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2322,23 +2321,23 @@
         <v>168</v>
       </c>
       <c r="C47" s="4">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H47" s="5"/>
       <c r="L47" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2346,23 +2345,23 @@
         <v>168</v>
       </c>
       <c r="C48" s="4">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>171</v>
+        <v>72</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H48" s="5"/>
       <c r="L48" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2370,23 +2369,23 @@
         <v>168</v>
       </c>
       <c r="C49" s="4">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>77</v>
+        <v>171</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H49" s="5"/>
       <c r="L49" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2394,35 +2393,34 @@
         <v>168</v>
       </c>
       <c r="C50" s="4">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H50" s="5"/>
       <c r="L50" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B51" s="8"/>
       <c r="C51" s="4">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>40</v>
@@ -2435,31 +2433,32 @@
       </c>
       <c r="H51" s="5"/>
       <c r="L51" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="B52" s="8"/>
       <c r="C52" s="4">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H52" s="5"/>
       <c r="L52" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2467,10 +2466,10 @@
         <v>168</v>
       </c>
       <c r="C53" s="4">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>40</v>
@@ -2479,109 +2478,109 @@
         <v>9</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H53" s="5"/>
       <c r="L53" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B54" s="8"/>
       <c r="C54" s="4">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H54" s="5"/>
       <c r="L54" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="B55" s="8"/>
       <c r="C55" s="4">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H55" s="5"/>
       <c r="L55" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B56" s="8"/>
       <c r="C56" s="4">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H56" s="5"/>
       <c r="L56" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="B57" s="8"/>
       <c r="C57" s="4">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>43</v>
       </c>
       <c r="H57" s="5"/>
       <c r="L57" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2589,23 +2588,23 @@
         <v>168</v>
       </c>
       <c r="C58" s="4">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>173</v>
+        <v>91</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>43</v>
       </c>
       <c r="H58" s="5"/>
       <c r="L58" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2613,23 +2612,23 @@
         <v>168</v>
       </c>
       <c r="C59" s="4">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>94</v>
+        <v>173</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>43</v>
       </c>
       <c r="H59" s="5"/>
       <c r="L59" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2637,21 +2636,23 @@
         <v>168</v>
       </c>
       <c r="C60" s="4">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G60" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="H60" s="5"/>
       <c r="L60" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2659,21 +2660,21 @@
         <v>168</v>
       </c>
       <c r="C61" s="4">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
       <c r="L61" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2681,24 +2682,21 @@
         <v>168</v>
       </c>
       <c r="C62" s="4">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
       <c r="L62" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="R62" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2706,21 +2704,21 @@
         <v>168</v>
       </c>
       <c r="C63" s="4">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="L63" s="6" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="R63" s="4" t="s">
         <v>102</v>
@@ -2731,21 +2729,24 @@
         <v>168</v>
       </c>
       <c r="C64" s="4">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="L64" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
+      </c>
+      <c r="R64" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2753,21 +2754,21 @@
         <v>168</v>
       </c>
       <c r="C65" s="4">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="L65" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2775,10 +2776,10 @@
         <v>168</v>
       </c>
       <c r="C66" s="4">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>40</v>
@@ -2789,81 +2790,76 @@
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
       <c r="L66" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B67" s="8"/>
       <c r="C67" s="4">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>162</v>
+        <v>109</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G67" s="5"/>
       <c r="H67" s="5"/>
       <c r="L67" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="B68" s="8"/>
       <c r="C68" s="4">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>111</v>
+        <v>162</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G68" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="H68" s="5"/>
       <c r="L68" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B69" s="8" t="s">
-        <v>168</v>
-      </c>
       <c r="C69" s="4">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>134</v>
+        <v>40</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>150</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G69" s="5"/>
       <c r="H69" s="5"/>
       <c r="L69" s="6" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2874,25 +2870,23 @@
         <v>168</v>
       </c>
       <c r="C70" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>134</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>131</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="H70" s="5"/>
       <c r="L70" s="6" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
     </row>
     <row r="71" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2903,10 +2897,10 @@
         <v>168</v>
       </c>
       <c r="C71" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>134</v>
@@ -2915,14 +2909,13 @@
         <v>6</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H71" s="5"/>
+        <v>132</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="L71" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="R71" s="4" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2933,28 +2926,26 @@
         <v>168</v>
       </c>
       <c r="C72" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>134</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H72" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="I72" s="4" t="s">
-        <v>145</v>
-      </c>
+      <c r="H72" s="5"/>
       <c r="L72" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
+      </c>
+      <c r="R72" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2965,19 +2956,19 @@
         <v>168</v>
       </c>
       <c r="C73" s="4">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>134</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>132</v>
+        <v>18</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>131</v>
@@ -2986,7 +2977,7 @@
         <v>145</v>
       </c>
       <c r="L73" s="6" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2997,10 +2988,10 @@
         <v>168</v>
       </c>
       <c r="C74" s="4">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>134</v>
@@ -3008,15 +2999,17 @@
       <c r="F74" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G74" s="5"/>
+      <c r="G74" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="H74" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="J74" s="4" t="s">
-        <v>18</v>
+      <c r="I74" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="L74" s="6" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -3027,23 +3020,26 @@
         <v>168</v>
       </c>
       <c r="C75" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>134</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H75" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L75" s="6" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -3054,10 +3050,10 @@
         <v>168</v>
       </c>
       <c r="C76" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>134</v>
@@ -3070,7 +3066,7 @@
       </c>
       <c r="H76" s="5"/>
       <c r="L76" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="77" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -3081,28 +3077,23 @@
         <v>168</v>
       </c>
       <c r="C77" s="4">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>134</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="J77" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H77" s="5"/>
       <c r="L77" s="6" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="78" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -3113,25 +3104,28 @@
         <v>168</v>
       </c>
       <c r="C78" s="4">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>134</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="H78" s="5" t="s">
         <v>131</v>
       </c>
+      <c r="J78" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L78" s="6" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -3142,31 +3136,25 @@
         <v>168</v>
       </c>
       <c r="C79" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>134</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>132</v>
+        <v>18</v>
       </c>
       <c r="H79" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="I79" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="J79" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L79" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -3177,10 +3165,10 @@
         <v>168</v>
       </c>
       <c r="C80" s="4">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>134</v>
@@ -3189,11 +3177,19 @@
         <v>8</v>
       </c>
       <c r="G80" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="J80" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H80" s="5"/>
       <c r="L80" s="6" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -3204,10 +3200,10 @@
         <v>168</v>
       </c>
       <c r="C81" s="4">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>134</v>
@@ -3215,18 +3211,12 @@
       <c r="F81" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G81" s="5"/>
-      <c r="H81" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="I81" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="J81" s="4" t="s">
+      <c r="G81" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="H81" s="5"/>
       <c r="L81" s="6" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -3237,41 +3227,88 @@
         <v>168</v>
       </c>
       <c r="C82" s="4">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="E82" s="5" t="s">
         <v>134</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G82" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G82" s="5"/>
       <c r="H82" s="5" t="s">
         <v>131</v>
       </c>
+      <c r="I82" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L82" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C83" s="4">
+        <v>25</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="L83" s="6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="8"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5"/>
-      <c r="H83" s="5"/>
-    </row>
     <row r="84" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="5"/>
-      <c r="H84" s="5"/>
+      <c r="A84" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C84" s="4">
+        <v>82</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H84" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="L84" s="10" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="85" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D85" s="5"/>
@@ -3546,11 +3583,18 @@
       <c r="G123" s="5"/>
       <c r="H123" s="5"/>
     </row>
-    <row r="1048519" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1048519" s="7"/>
+    <row r="124" spans="4:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D124" s="5"/>
+      <c r="E124" s="5"/>
+      <c r="F124" s="5"/>
+      <c r="G124" s="5"/>
+      <c r="H124" s="5"/>
+    </row>
+    <row r="1048520" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1048520" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V83" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A2:V84" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="6" showButton="0"/>
     <filterColumn colId="7" showButton="0"/>
     <filterColumn colId="8" showButton="0"/>
@@ -3562,40 +3606,40 @@
     <filterColumn colId="15" showButton="0"/>
   </autoFilter>
   <mergeCells count="3">
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:Q1"/>
-    <mergeCell ref="L29:Q29"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:Q2"/>
+    <mergeCell ref="L30:Q30"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:B20 A22:B1048576">
+  <conditionalFormatting sqref="A2:B21 A23:B1048576">
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="YES">
-      <formula>NOT(ISERROR(SEARCH("YES",A1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("YES",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E20 E22:E1048576">
+  <conditionalFormatting sqref="E2:E21 E23:E1048576">
     <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="strength">
-      <formula>NOT(ISERROR(SEARCH("strength",E1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("strength",E2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="OCR">
-      <formula>NOT(ISERROR(SEARCH("OCR",E1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OCR",E2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="Run">
-      <formula>NOT(ISERROR(SEARCH("Run",E1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Run",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21:B21">
+  <conditionalFormatting sqref="A22:B22">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="YES">
-      <formula>NOT(ISERROR(SEARCH("YES",A21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("YES",A22)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="E22">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="strength">
-      <formula>NOT(ISERROR(SEARCH("strength",E21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("strength",E22)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="OCR">
-      <formula>NOT(ISERROR(SEARCH("OCR",E21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OCR",E22)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Run">
-      <formula>NOT(ISERROR(SEARCH("Run",E21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Run",E22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>